<commit_message>
Carry Select Adder code added
</commit_message>
<xml_diff>
--- a/by Subject/Hierarchy/Adder2/adder2_README.xlsx
+++ b/by Subject/Hierarchy/Adder2/adder2_README.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Specifications\ATE Test Equipment\Harrison Warke\Verilog_HDLBits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Specifications\ATE Test Equipment\Harrison Warke\Verilog_HDLBits\by Subject\Hierarchy\Adder2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4376E0D-FA5F-45A6-86FA-C3F9E8ECAE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A576A5-E29C-41E8-B7C7-12F940204344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="-16308" windowWidth="29016" windowHeight="15696" xr2:uid="{A1D08BBE-7EFC-481F-973D-2B91297FF584}"/>
+    <workbookView xWindow="-11400" yWindow="-16308" windowWidth="25416" windowHeight="15252" xr2:uid="{A1D08BBE-7EFC-481F-973D-2B91297FF584}"/>
   </bookViews>
   <sheets>
     <sheet name="module fadd" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>add16 module</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>1-bit full adder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instantiate two copies of add16 (provided). </t>
   </si>
 </sst>
 </file>
@@ -331,29 +334,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -366,19 +357,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -388,6 +391,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -776,7 +782,7 @@
   <dimension ref="B1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -791,61 +797,63 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="130.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="10" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="19"/>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="17"/>
       <c r="H4" s="18"/>
       <c r="I4" s="19"/>
-      <c r="J4" s="16"/>
+      <c r="J4" s="20" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>

</xml_diff>